<commit_message>
Made excel file path in config file
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/testdata.xlsx
+++ b/src/test/resources/Exceldata/testdata.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aswi1\eclipse-workspace\dsAlgo\src\test\resources\Exceldata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A25D66-C371-487E-B887-FE67F55CF296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D89B5A53-ECC3-4583-95F8-9D5767EAECDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="signin" sheetId="1" r:id="rId1"/>
     <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:D6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -415,7 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -506,7 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9432A9A0-530D-4EB9-BB11-570827F1063D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Test ran with reports
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/testdata.xlsx
+++ b/src/test/resources/Exceldata/testdata.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D89B5A53-ECC3-4583-95F8-9D5767EAECDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{32276A89-2EE8-4C19-ACE6-69490D5DCC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="signin" sheetId="1" r:id="rId1"/>
     <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D6"/>
+  <oleSize ref="A1:M11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -411,7 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -502,7 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9432A9A0-530D-4EB9-BB11-570827F1063D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>